<commit_message>
fix sorted dic err=>STABLE
</commit_message>
<xml_diff>
--- a/recommendApi/media/cvsDbData1.xlsx
+++ b/recommendApi/media/cvsDbData1.xlsx
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>6391c91c695c9b70a0bd8835</t>
+          <t>6391d83460c5c272169dac4d</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>game development unitygame development unity</t>
+          <t>nodejs nodejs node jsnodejs nodejs node js</t>
         </is>
       </c>
     </row>

</xml_diff>